<commit_message>
Proper Column Name formatting
Generated files column name for Fs changed into 'SamplingFrequency'
</commit_message>
<xml_diff>
--- a/Measurements/ECG_1.xlsx
+++ b/Measurements/ECG_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergi\Documents\GitHub\IBES\Measurements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCAC7D8C-B19D-4776-810C-0337DB0DB002}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33DEA33C-8DFA-4DEB-B788-2280967632FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,10 +27,10 @@
     <t>time</t>
   </si>
   <si>
-    <t>Sampling Frequency</t>
+    <t>ECG</t>
   </si>
   <si>
-    <t>ECG</t>
+    <t>SamplingFrequency</t>
   </si>
 </sst>
 </file>
@@ -408,8 +408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A974" workbookViewId="0">
-      <selection activeCell="C1005" sqref="C1005"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,10 +419,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>